<commit_message>
Updated example to show use of the previousRow in the ExcelFixtureRowHandler API.
</commit_message>
<xml_diff>
--- a/fixture/src/main/java/org/isisaddons/module/excel/fixture/scripts/ToDoItems.xlsx
+++ b/fixture/src/main/java/org/isisaddons/module/excel/fixture/scripts/ToDoItems.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
   <si>
     <t>description</t>
   </si>
@@ -450,30 +450,30 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomRight" activeCell="D2" sqref="D2:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
       </c>
       <c r="D1" t="s">
         <v>27</v>
@@ -484,13 +484,13 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" t="s">
-        <v>23</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -500,14 +500,9 @@
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" t="s">
+      <c r="A3" s="1"/>
+      <c r="C3" t="s">
         <v>5</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" t="s">
-        <v>23</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -517,14 +512,9 @@
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" t="s">
+      <c r="A4" s="1"/>
+      <c r="C4" t="s">
         <v>6</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" t="s">
-        <v>23</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -534,14 +524,12 @@
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" t="s">
+      <c r="A5" s="1"/>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s">
         <v>7</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" t="s">
-        <v>24</v>
       </c>
       <c r="D5">
         <v>6</v>
@@ -551,109 +539,97 @@
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" t="s">
+      <c r="A6" s="1"/>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
         <v>8</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" t="s">
-        <v>25</v>
       </c>
       <c r="D6">
         <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" t="s">
+      <c r="A7" s="1"/>
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" t="s">
         <v>9</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" t="s">
-        <v>26</v>
       </c>
       <c r="D7">
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" t="s">
+      <c r="A8" s="1"/>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
         <v>10</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" t="s">
-        <v>24</v>
       </c>
       <c r="D8">
         <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" t="s">
-        <v>17</v>
-      </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" t="s">
+      <c r="A10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
         <v>12</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" t="s">
-        <v>19</v>
       </c>
       <c r="D10">
         <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" t="s">
+      <c r="A11" s="1"/>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" t="s">
         <v>13</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" t="s">
-        <v>20</v>
       </c>
       <c r="D11">
         <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" t="s">
+      <c r="A12" s="1"/>
+      <c r="B12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" t="s">
         <v>14</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" t="s">
-        <v>21</v>
       </c>
       <c r="D12">
         <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" t="s">
+      <c r="A13" s="1"/>
+      <c r="B13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" t="s">
         <v>15</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ExcelFixture now has value semantics, and using the new MultipleExecutionStrategy.  Updated the demo app to illustrate its use, updated the README.
Also:
- converted to use AppManifest
</commit_message>
<xml_diff>
--- a/fixture/src/main/java/org/isisaddons/module/excel/fixture/scripts/ToDoItems.xlsx
+++ b/fixture/src/main/java/org/isisaddons/module/excel/fixture/scripts/ToDoItems.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\isisaddons\isis-module-excel\fixture\src\main\java\org\isisaddons\module\excel\fixture\scripts\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="30" windowWidth="19155" windowHeight="10305"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>description</t>
   </si>
@@ -51,40 +56,7 @@
     <t>Sharpen knives</t>
   </si>
   <si>
-    <t>Write to penpal</t>
-  </si>
-  <si>
-    <t>Write blog post</t>
-  </si>
-  <si>
-    <t>Organize brown bag</t>
-  </si>
-  <si>
-    <t>Submit conference session</t>
-  </si>
-  <si>
-    <t>Stage Isis release</t>
-  </si>
-  <si>
     <t>Domestic</t>
-  </si>
-  <si>
-    <t>Other</t>
-  </si>
-  <si>
-    <t>Professional</t>
-  </si>
-  <si>
-    <t>Marketing</t>
-  </si>
-  <si>
-    <t>Consulting</t>
-  </si>
-  <si>
-    <t>Education</t>
-  </si>
-  <si>
-    <t>OpenSource</t>
   </si>
   <si>
     <t>Shopping</t>
@@ -105,7 +77,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -156,6 +128,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -203,7 +178,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -238,7 +213,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -453,7 +428,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D2" sqref="D2:D4"/>
+      <selection pane="bottomRight" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -476,7 +451,7 @@
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>3</v>
@@ -484,10 +459,10 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -526,7 +501,7 @@
     <row r="5" spans="1:5">
       <c r="A5" s="1"/>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
@@ -541,7 +516,7 @@
     <row r="6" spans="1:5">
       <c r="A6" s="1"/>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
@@ -553,7 +528,7 @@
     <row r="7" spans="1:5">
       <c r="A7" s="1"/>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
         <v>9</v>
@@ -565,7 +540,7 @@
     <row r="8" spans="1:5">
       <c r="A8" s="1"/>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s">
         <v>10</v>
@@ -575,62 +550,19 @@
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" t="s">
-        <v>11</v>
-      </c>
+      <c r="A9" s="1"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10">
-        <v>7</v>
-      </c>
+      <c r="A10" s="1"/>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="1"/>
-      <c r="B11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11">
-        <v>14</v>
-      </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="1"/>
-      <c r="B12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12">
-        <v>21</v>
-      </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="1"/>
-      <c r="B13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" t="s">
-        <v>15</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Makes sheet name and row number available to handler
When the handler implements ExcelMetaDataEnabled sheet name and row number of the row to handle are available.
</commit_message>
<xml_diff>
--- a/fixture/src/main/java/org/isisaddons/module/excel/fixture/scripts/ToDoItems.xlsx
+++ b/fixture/src/main/java/org/isisaddons/module/excel/fixture/scripts/ToDoItems.xlsx
@@ -1,27 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\isisaddons\isis-module-excel\fixture\src\main\java\org\isisaddons\module\excel\fixture\scripts\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="19155" windowHeight="10305"/>
+    <workbookView xWindow="480" yWindow="40" windowWidth="19160" windowHeight="10300" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ExcelModuleDemoToDoItem" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="18">
   <si>
     <t>description</t>
   </si>
@@ -72,13 +72,16 @@
   </si>
   <si>
     <t>daysFromToday</t>
+  </si>
+  <si>
+    <t>Another Item</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -178,7 +181,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -213,7 +216,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -424,20 +427,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="2"/>
+    <col min="5" max="5" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -474,7 +477,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" ht="15">
       <c r="A3" s="1"/>
       <c r="C3" t="s">
         <v>5</v>
@@ -486,7 +489,7 @@
         <v>1.75</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" ht="15">
       <c r="A4" s="1"/>
       <c r="C4" t="s">
         <v>6</v>
@@ -498,7 +501,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" ht="15">
       <c r="A5" s="1"/>
       <c r="B5" t="s">
         <v>13</v>
@@ -513,7 +516,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" ht="15">
       <c r="A6" s="1"/>
       <c r="B6" t="s">
         <v>14</v>
@@ -525,7 +528,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" ht="15">
       <c r="A7" s="1"/>
       <c r="B7" t="s">
         <v>15</v>
@@ -537,7 +540,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" ht="15">
       <c r="A8" s="1"/>
       <c r="B8" t="s">
         <v>13</v>
@@ -549,47 +552,166 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" ht="15">
       <c r="A9" s="1"/>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" ht="15">
       <c r="A10" s="1"/>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" ht="15">
       <c r="A11" s="1"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" ht="15">
       <c r="A12" s="1"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" ht="15">
       <c r="A13" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15">
+      <c r="A3" s="1"/>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15">
+      <c r="A4" s="1"/>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15">
+      <c r="A5" s="1"/>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15">
+      <c r="A6" s="1"/>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15">
+      <c r="A7" s="1"/>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15">
+      <c r="A8" s="1"/>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15">
+      <c r="A5" s="1"/>
+    </row>
+    <row r="6" spans="1:3" ht="15">
+      <c r="A6" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>